<commit_message>
correct some comment typos, added day margin rate calucation for 25% day rate
</commit_message>
<xml_diff>
--- a/marginrates.xlsx
+++ b/marginrates.xlsx
@@ -426,7 +426,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>$3,300.00</t>
+          <t>$0.00</t>
         </is>
       </c>
     </row>
@@ -490,7 +490,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>$4,125.00</t>
+          <t>$0.00</t>
         </is>
       </c>
     </row>
@@ -522,7 +522,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>$1,952.50</t>
+          <t>$0.00</t>
         </is>
       </c>
     </row>
@@ -554,7 +554,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>$3,300.00</t>
+          <t>$0.00</t>
         </is>
       </c>
     </row>
@@ -586,7 +586,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>$330.00</t>
+          <t>$0.00</t>
         </is>
       </c>
     </row>
@@ -618,7 +618,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>$412.50</t>
+          <t>$0.00</t>
         </is>
       </c>
     </row>
@@ -650,7 +650,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>$195.25</t>
+          <t>$0.00</t>
         </is>
       </c>
     </row>
@@ -682,7 +682,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>$330.00</t>
+          <t>$0.00</t>
         </is>
       </c>
     </row>
@@ -874,7 +874,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>$0.00</t>
+          <t>$990.00</t>
         </is>
       </c>
     </row>
@@ -906,7 +906,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>$0.00</t>
+          <t>$1,485.00</t>
         </is>
       </c>
     </row>
@@ -938,7 +938,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>$0.00</t>
+          <t>$852.50</t>
         </is>
       </c>
     </row>
@@ -970,7 +970,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>$0.00</t>
+          <t>$1,251.50</t>
         </is>
       </c>
     </row>
@@ -1002,7 +1002,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>$0.00</t>
+          <t>$2,200.00</t>
         </is>
       </c>
     </row>
@@ -1066,7 +1066,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>$0.00</t>
+          <t>$825.00</t>
         </is>
       </c>
     </row>
@@ -1098,7 +1098,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>$0.00</t>
+          <t>$2,475.00</t>
         </is>
       </c>
     </row>
@@ -1130,7 +1130,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>$0.00</t>
+          <t>$1,375.00</t>
         </is>
       </c>
     </row>
@@ -1162,7 +1162,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>$0.00</t>
+          <t>$626.00</t>
         </is>
       </c>
     </row>
@@ -1194,7 +1194,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>$0.00</t>
+          <t>$1,100.00</t>
         </is>
       </c>
     </row>
@@ -1322,7 +1322,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>$0.00</t>
+          <t>$3,300.00</t>
         </is>
       </c>
     </row>
@@ -1354,7 +1354,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>$0.00</t>
+          <t>$6,875.00</t>
         </is>
       </c>
     </row>
@@ -1386,7 +1386,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>$0.00</t>
+          <t>$1,100.00</t>
         </is>
       </c>
     </row>
@@ -1418,7 +1418,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>$0.00</t>
+          <t>$1,952.50</t>
         </is>
       </c>
     </row>
@@ -1450,7 +1450,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>$0.00</t>
+          <t>$467.50</t>
         </is>
       </c>
     </row>
@@ -1482,7 +1482,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>$0.00</t>
+          <t>$344.00</t>
         </is>
       </c>
     </row>
@@ -1546,7 +1546,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>$0.00</t>
+          <t>$5,032.50</t>
         </is>
       </c>
     </row>
@@ -1578,7 +1578,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>$0.00</t>
+          <t>$4,950.00</t>
         </is>
       </c>
     </row>
@@ -1610,7 +1610,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>$0.00</t>
+          <t>$2,062.50</t>
         </is>
       </c>
     </row>
@@ -1642,7 +1642,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>$0.00</t>
+          <t>$24,200.00</t>
         </is>
       </c>
     </row>
@@ -1674,7 +1674,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>$0.00</t>
+          <t>$2,475.00</t>
         </is>
       </c>
     </row>

</xml_diff>